<commit_message>
Edit project sprint report
</commit_message>
<xml_diff>
--- a/TeamHJSReport 1.0.xlsx
+++ b/TeamHJSReport 1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkfan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkfan/PycharmProjects/19S-Stevens-SSW-555/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B371F2DF-FB07-ED4C-8F85-386986D7E5BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695820D9-DF53-BC48-87FD-555C79D706C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="252">
   <si>
     <t>Compare marriage date to birth date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -818,10 +818,16 @@
     <t>JK</t>
   </si>
   <si>
-    <t>Some of the test cases contained multiple boundary conditions, which may cause inaccurate test result. Besides, we didn't do well in branch management at first. We believe we should avoid these issues in future sprints.</t>
-  </si>
-  <si>
-    <t>We build a good project structure for both application and testing. All codes are easy to read and reuse.</t>
+    <t>Maintain a good project structure for both application and testing.</t>
+  </si>
+  <si>
+    <t>All codes are easy to read and reuse.</t>
+  </si>
+  <si>
+    <t>Some of the test cases may contain multiple boundary conditions.</t>
+  </si>
+  <si>
+    <t>Branch and  commit management sometimes run into chaos.</t>
   </si>
 </sst>
 </file>
@@ -959,7 +965,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1005,6 +1011,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2843,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3269,65 +3278,69 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B36" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-    </row>
-    <row r="38" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+    </row>
+    <row r="38" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
+        <v>250</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
+      <c r="B39" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B40" s="21"/>
@@ -3340,9 +3353,12 @@
       <c r="I40" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B35:I37"/>
-    <mergeCell ref="B38:I40"/>
+  <mergeCells count="5">
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B39:I39"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3615,7 +3631,7 @@
     <col min="1" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -3663,7 +3679,7 @@
     <col min="1" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Code for demo of sprint 1
</commit_message>
<xml_diff>
--- a/TeamHJSReport 1.0.xlsx
+++ b/TeamHJSReport 1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkfan/PycharmProjects/19S-Stevens-SSW-555/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695820D9-DF53-BC48-87FD-555C79D706C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827489C2-0F11-384D-B5AE-A41BE3DC2AC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2852,7 +2852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>

</xml_diff>